<commit_message>
changement tableau de synthèse
</commit_message>
<xml_diff>
--- a/image/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2022 (1).xlsx
+++ b/image/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2022 (1).xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etienne\travail\git\portfolio\image\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA00ED0-50FA-4506-BEC9-C5A4A9A26C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$31</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,9 +22,6 @@
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
   <si>
-    <t>SESSION 2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
@@ -47,29 +38,6 @@
   </si>
   <si>
     <t>▢ SISR</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">▢ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>SLAM</t>
-    </r>
-  </si>
-  <si>
-    <t>Adresse URL du portfolio : C:/Documents/GitHub/Portfolio/portfolio.html</t>
   </si>
   <si>
     <t>Compétences mises en œuvre
@@ -148,9 +116,6 @@
     <t>Projet Personnel : projet en java permettant de gérer une liste d'employé de ligues en ayant un administrateur par ligue et un administrateur global. (code source, MCD, compte rendu, arborescence de l'application, historique de GitHub)</t>
   </si>
   <si>
-    <t xml:space="preserve">Veille informationnelle sur le machine learning </t>
-  </si>
-  <si>
     <t>Projet Parking : Création d'un site pour réserver des places de parking, avec point de vu administrateur : gérer les utilisateurs et les réservations, et utilisateur : file d'attente et visions des précèdentes places prise. (code source, MCD, arborescence de l'application, historique GitHub)</t>
   </si>
   <si>
@@ -166,9 +131,6 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>Ajout de fonctionnalité à un site internet interne de l'entreprise afin d'aider les potentielles demande pouvant être faites aux developpeur, par rapport aux problèmes rencontrés par les clients sur le site internet de l'entreprise. (utilisation du framework Spring et Angular et d'Oracle.) (Documentation)</t>
-  </si>
-  <si>
     <t>03/01/2023 au 03/02/2023</t>
   </si>
   <si>
@@ -176,16 +138,31 @@
   </si>
   <si>
     <t>12/08/2022 au 03/04/2023</t>
+  </si>
+  <si>
+    <t>X SLAM</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://etihaine.github.io/portfolio/</t>
+  </si>
+  <si>
+    <t>SESSION 2023</t>
+  </si>
+  <si>
+    <t>Veille informationnelle sur le machine learning/ IA</t>
+  </si>
+  <si>
+    <t>Ajout de fonctionnalités à un site internet interne de l'entreprise afin d'aider les demandes potentielles  pouvant être faites aux developpeurs, par rapport aux problèmes rencontrés par les clients sur le site internet de l'entreprise. (utilisation du framework Spring et Angular et d'Oracle.) (Documentation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -250,19 +227,20 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FF70AD47"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -664,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -717,10 +695,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -732,9 +707,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -759,48 +773,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Euro" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -859,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -891,27 +875,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -943,24 +909,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1136,17 +1084,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" style="1" customWidth="1"/>
@@ -1155,125 +1103,125 @@
     <col min="44" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="31"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="43"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1">
+      <c r="A4" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1">
+      <c r="A5" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1">
+      <c r="A6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="B6" s="31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1">
+      <c r="A7" s="23"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="D7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="E7" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="H7" s="21" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1311,17 +1259,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A8" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1358,16 +1306,16 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
-        <v>26</v>
+      <c r="F9" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -1407,25 +1355,25 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="60" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>26</v>
+      <c r="C10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10"/>
@@ -1464,25 +1412,25 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="107.25" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>26</v>
+      <c r="C11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11"/>
@@ -1521,20 +1469,20 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="15" t="s">
-        <v>26</v>
+      <c r="H12" s="45" t="s">
+        <v>23</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1572,18 +1520,18 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="96.75" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>26</v>
+      <c r="E13" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -1623,7 +1571,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14"/>
@@ -1668,7 +1616,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14"/>
@@ -1713,7 +1661,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14"/>
@@ -1758,7 +1706,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
       <c r="C17" s="14"/>
@@ -1803,15 +1751,17 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A18" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1848,17 +1798,23 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1895,21 +1851,13 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>33</v>
-      </c>
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
       <c r="I20"/>
@@ -1948,7 +1896,7 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="8"/>
       <c r="C21" s="14"/>
@@ -1993,7 +1941,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
       <c r="C22" s="14"/>
@@ -2038,15 +1986,17 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A23" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="30"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2083,13 +2033,25 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="95.25" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
       <c r="I24"/>
@@ -2128,14 +2090,18 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="B25" s="8"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="H25" s="15"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -2173,7 +2139,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
       <c r="C26" s="14"/>
@@ -2218,17 +2184,15 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A27" s="9"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="15"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2265,25 +2229,13 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>26</v>
-      </c>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
       <c r="I28"/>
@@ -2322,18 +2274,14 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>37</v>
-      </c>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A29" s="9"/>
       <c r="B29" s="8"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="G29" s="14"/>
       <c r="H29" s="15"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -2371,15 +2319,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2416,15 +2364,15 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="15">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2461,251 +2409,71 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
-      <c r="AP32"/>
-      <c r="AQ32"/>
-    </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-    </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34"/>
-      <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
-      <c r="AJ34"/>
-      <c r="AK34"/>
-      <c r="AL34"/>
-      <c r="AM34"/>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
-      <c r="AQ34"/>
-    </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-    </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:43" customFormat="1"/>
+    <row r="33" customFormat="1"/>
+    <row r="34" customFormat="1"/>
+    <row r="35" customFormat="1"/>
+    <row r="36" customFormat="1"/>
+    <row r="37" customFormat="1"/>
+    <row r="38" customFormat="1"/>
+    <row r="39" customFormat="1"/>
+    <row r="40" customFormat="1"/>
+    <row r="41" customFormat="1"/>
+    <row r="42" customFormat="1"/>
+    <row r="43" customFormat="1"/>
+    <row r="44" customFormat="1"/>
+    <row r="45" customFormat="1"/>
+    <row r="46" customFormat="1"/>
+    <row r="47" customFormat="1"/>
+    <row r="48" customFormat="1"/>
+    <row r="49" customFormat="1"/>
+    <row r="50" customFormat="1"/>
+    <row r="51" customFormat="1"/>
+    <row r="52" customFormat="1"/>
+    <row r="53" customFormat="1"/>
+    <row r="54" customFormat="1"/>
+    <row r="55" customFormat="1"/>
+    <row r="56" customFormat="1"/>
+    <row r="57" customFormat="1"/>
+    <row r="58" customFormat="1"/>
+    <row r="59" customFormat="1"/>
+    <row r="60" customFormat="1"/>
+    <row r="61" customFormat="1"/>
+    <row r="62" customFormat="1"/>
+    <row r="63" customFormat="1"/>
+    <row r="64" customFormat="1"/>
+    <row r="65" customFormat="1"/>
+    <row r="66" customFormat="1"/>
+    <row r="67" customFormat="1"/>
+    <row r="68" customFormat="1"/>
+    <row r="69" customFormat="1"/>
+    <row r="70" customFormat="1"/>
+    <row r="71" customFormat="1"/>
+    <row r="72" customFormat="1"/>
+    <row r="73" customFormat="1"/>
+    <row r="74" customFormat="1"/>
+    <row r="75" customFormat="1"/>
+    <row r="76" customFormat="1"/>
+    <row r="77" customFormat="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="47" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>